<commit_message>
Adjusts scale and ticks
</commit_message>
<xml_diff>
--- a/special-ed/special-ed.xlsx
+++ b/special-ed/special-ed.xlsx
@@ -23,6 +23,9 @@
     <t>value</t>
   </si>
   <si>
+    <t>headline</t>
+  </si>
+  <si>
     <t>Funding</t>
   </si>
   <si>
@@ -32,25 +35,16 @@
     <t>funding per student</t>
   </si>
   <si>
-    <t>headline</t>
+    <t>headli ne here</t>
   </si>
   <si>
     <t>2014</t>
   </si>
   <si>
-    <t>headli ne here</t>
+    <t>subhed</t>
   </si>
   <si>
     <t>507406358.99</t>
-  </si>
-  <si>
-    <t>subhed</t>
-  </si>
-  <si>
-    <t>42743</t>
-  </si>
-  <si>
-    <t>11871.0984</t>
   </si>
   <si>
     <t>footnote</t>
@@ -65,10 +59,25 @@
     <t>NPR</t>
   </si>
   <si>
-    <t>2015</t>
+    <t>header_one</t>
   </si>
   <si>
-    <t>header_one</t>
+    <t>As the special education population in CPS went up...</t>
+  </si>
+  <si>
+    <t>header_two</t>
+  </si>
+  <si>
+    <t>the funding for special education programs went down.</t>
+  </si>
+  <si>
+    <t>42743</t>
+  </si>
+  <si>
+    <t>11871.0984</t>
+  </si>
+  <si>
+    <t>2015</t>
   </si>
   <si>
     <t>495813056.47</t>
@@ -78,9 +87,6 @@
   </si>
   <si>
     <t>12298.47591</t>
-  </si>
-  <si>
-    <t>As the special education population in CPS went up...</t>
   </si>
   <si>
     <t>2016</t>
@@ -93,12 +99,6 @@
   </si>
   <si>
     <t>10887.05119</t>
-  </si>
-  <si>
-    <t>header_two</t>
-  </si>
-  <si>
-    <t>the funding for special education programs went down.</t>
   </si>
 </sst>
 </file>
@@ -155,10 +155,13 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
@@ -168,14 +171,11 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
@@ -218,472 +218,472 @@
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
     <row r="2" ht="33.0" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>6</v>
+      <c r="A2" s="4" t="s">
+        <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>8</v>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
     </row>
     <row r="3" ht="33.0" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>10</v>
+      <c r="A3" s="4" t="s">
+        <v>9</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
     </row>
     <row r="4" ht="33.0" customHeight="1">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+    </row>
+    <row r="5" ht="33.0" customHeight="1">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+    </row>
+    <row r="6" ht="33.0" customHeight="1">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-    </row>
-    <row r="5" ht="33.0" customHeight="1">
-      <c r="A5" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-    </row>
-    <row r="6" ht="33.0" customHeight="1">
-      <c r="A6" s="5" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+    </row>
+    <row r="7" ht="33.0" customHeight="1">
+      <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-    </row>
-    <row r="7" ht="33.0" customHeight="1">
-      <c r="A7" s="5" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+    </row>
+    <row r="8" ht="33.0" customHeight="1">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
-    </row>
-    <row r="8" ht="33.0" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
     </row>
     <row r="9" ht="33.0" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
     </row>
     <row r="10" ht="33.0" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
     </row>
     <row r="11" ht="33.0" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="7"/>
-      <c r="Z11" s="7"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
     </row>
     <row r="12" ht="33.0" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="7"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
     </row>
     <row r="13" ht="33.0" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
-      <c r="Z13" s="7"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
     </row>
     <row r="14" ht="33.0" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
     </row>
     <row r="15" ht="33.0" customHeight="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="7"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
     </row>
     <row r="16" ht="33.0" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="7"/>
-      <c r="Z16" s="7"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -705,771 +705,779 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>7</v>
+      <c r="A2" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>9</v>
+      <c r="B2" s="9" t="s">
+        <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>11</v>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="6" t="s">
+      <c r="B3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="D3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="C4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="G5">
+        <f>(D2+D3+D4)/3</f>
+        <v>11685.54183</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="H7">
+        <f>400000000/G5</f>
+        <v>34230.33401</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
     </row>
     <row r="24">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
     </row>
     <row r="26">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
     </row>
     <row r="39">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
     </row>
     <row r="40">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
     </row>
     <row r="41">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
     </row>
     <row r="42">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
     </row>
     <row r="43">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
     </row>
     <row r="44">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
     </row>
     <row r="45">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
     </row>
     <row r="46">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
     </row>
     <row r="47">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
     </row>
     <row r="48">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
     </row>
     <row r="49">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
     </row>
     <row r="50">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
     </row>
     <row r="51">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
     </row>
     <row r="52">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
     </row>
     <row r="53">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
     </row>
     <row r="54">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
     </row>
     <row r="55">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
     </row>
     <row r="56">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
     </row>
     <row r="57">
-      <c r="A57" s="6"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
+      <c r="A57" s="7"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
     </row>
     <row r="58">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
     </row>
     <row r="59">
-      <c r="A59" s="6"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
     </row>
     <row r="60">
-      <c r="A60" s="6"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
     </row>
     <row r="61">
-      <c r="A61" s="6"/>
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6"/>
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
     </row>
     <row r="62">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6"/>
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
     </row>
     <row r="63">
-      <c r="A63" s="6"/>
-      <c r="B63" s="6"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
     </row>
     <row r="64">
-      <c r="A64" s="6"/>
-      <c r="B64" s="6"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="6"/>
-      <c r="E64" s="6"/>
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
     </row>
     <row r="65">
-      <c r="A65" s="6"/>
-      <c r="B65" s="6"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
-      <c r="E65" s="6"/>
+      <c r="A65" s="7"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
     </row>
     <row r="66">
-      <c r="A66" s="6"/>
-      <c r="B66" s="6"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
-      <c r="E66" s="6"/>
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
     </row>
     <row r="67">
-      <c r="A67" s="6"/>
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="6"/>
+      <c r="A67" s="7"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
     </row>
     <row r="68">
-      <c r="A68" s="6"/>
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
     </row>
     <row r="69">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
     </row>
     <row r="70">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="6"/>
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
     </row>
     <row r="71">
-      <c r="A71" s="6"/>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="6"/>
+      <c r="A71" s="7"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
     </row>
     <row r="72">
-      <c r="A72" s="6"/>
-      <c r="B72" s="6"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="6"/>
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
     </row>
     <row r="73">
-      <c r="A73" s="6"/>
-      <c r="B73" s="6"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
+      <c r="A73" s="7"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
     </row>
     <row r="74">
-      <c r="A74" s="6"/>
-      <c r="B74" s="6"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
+      <c r="A74" s="7"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
     </row>
     <row r="75">
-      <c r="A75" s="6"/>
-      <c r="B75" s="6"/>
-      <c r="C75" s="6"/>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
+      <c r="A75" s="7"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
     </row>
     <row r="76">
-      <c r="A76" s="6"/>
-      <c r="B76" s="6"/>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
+      <c r="A76" s="7"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
     </row>
     <row r="77">
-      <c r="A77" s="6"/>
-      <c r="B77" s="6"/>
-      <c r="C77" s="6"/>
-      <c r="D77" s="6"/>
-      <c r="E77" s="6"/>
+      <c r="A77" s="7"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
     </row>
     <row r="78">
-      <c r="A78" s="6"/>
-      <c r="B78" s="6"/>
-      <c r="C78" s="6"/>
-      <c r="D78" s="6"/>
-      <c r="E78" s="6"/>
+      <c r="A78" s="7"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
     </row>
     <row r="79">
-      <c r="A79" s="6"/>
-      <c r="B79" s="6"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
+      <c r="A79" s="7"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
     </row>
     <row r="80">
-      <c r="A80" s="6"/>
-      <c r="B80" s="6"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
     </row>
     <row r="81">
-      <c r="A81" s="6"/>
-      <c r="B81" s="6"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="6"/>
-      <c r="E81" s="6"/>
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
     </row>
     <row r="82">
-      <c r="A82" s="6"/>
-      <c r="B82" s="6"/>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="6"/>
+      <c r="A82" s="7"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
     </row>
     <row r="83">
-      <c r="A83" s="6"/>
-      <c r="B83" s="6"/>
-      <c r="C83" s="6"/>
-      <c r="D83" s="6"/>
-      <c r="E83" s="6"/>
+      <c r="A83" s="7"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
     </row>
     <row r="84">
-      <c r="A84" s="6"/>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
-      <c r="D84" s="6"/>
-      <c r="E84" s="6"/>
+      <c r="A84" s="7"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
     </row>
     <row r="85">
-      <c r="A85" s="6"/>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
-      <c r="D85" s="6"/>
-      <c r="E85" s="6"/>
+      <c r="A85" s="7"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
     </row>
     <row r="86">
-      <c r="A86" s="6"/>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
-      <c r="D86" s="6"/>
-      <c r="E86" s="6"/>
+      <c r="A86" s="7"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
     </row>
     <row r="87">
-      <c r="A87" s="6"/>
-      <c r="B87" s="6"/>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="6"/>
+      <c r="A87" s="7"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
     </row>
     <row r="88">
-      <c r="A88" s="6"/>
-      <c r="B88" s="6"/>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="6"/>
+      <c r="A88" s="7"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
     </row>
     <row r="89">
-      <c r="A89" s="6"/>
-      <c r="B89" s="6"/>
-      <c r="C89" s="6"/>
-      <c r="D89" s="6"/>
-      <c r="E89" s="6"/>
+      <c r="A89" s="7"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
     </row>
     <row r="90">
-      <c r="A90" s="6"/>
-      <c r="B90" s="6"/>
-      <c r="C90" s="6"/>
-      <c r="D90" s="6"/>
-      <c r="E90" s="6"/>
+      <c r="A90" s="7"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="7"/>
     </row>
     <row r="91">
-      <c r="A91" s="6"/>
-      <c r="B91" s="6"/>
-      <c r="C91" s="6"/>
-      <c r="D91" s="6"/>
-      <c r="E91" s="6"/>
+      <c r="A91" s="7"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
     </row>
     <row r="92">
-      <c r="A92" s="6"/>
-      <c r="B92" s="6"/>
-      <c r="C92" s="6"/>
-      <c r="D92" s="6"/>
-      <c r="E92" s="6"/>
+      <c r="A92" s="7"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
     </row>
     <row r="93">
-      <c r="A93" s="6"/>
-      <c r="B93" s="6"/>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="6"/>
+      <c r="A93" s="7"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
     </row>
     <row r="94">
-      <c r="A94" s="6"/>
-      <c r="B94" s="6"/>
-      <c r="C94" s="6"/>
-      <c r="D94" s="6"/>
-      <c r="E94" s="6"/>
+      <c r="A94" s="7"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
     </row>
     <row r="95">
-      <c r="A95" s="6"/>
-      <c r="B95" s="6"/>
-      <c r="C95" s="6"/>
-      <c r="D95" s="6"/>
-      <c r="E95" s="6"/>
+      <c r="A95" s="7"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
     </row>
     <row r="96">
-      <c r="A96" s="6"/>
-      <c r="B96" s="6"/>
-      <c r="C96" s="6"/>
-      <c r="D96" s="6"/>
-      <c r="E96" s="6"/>
+      <c r="A96" s="7"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="7"/>
     </row>
     <row r="97">
-      <c r="A97" s="6"/>
-      <c r="B97" s="6"/>
-      <c r="C97" s="6"/>
-      <c r="D97" s="6"/>
-      <c r="E97" s="6"/>
+      <c r="A97" s="7"/>
+      <c r="B97" s="7"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
     </row>
     <row r="98">
-      <c r="A98" s="6"/>
-      <c r="B98" s="6"/>
-      <c r="C98" s="6"/>
-      <c r="D98" s="6"/>
-      <c r="E98" s="6"/>
+      <c r="A98" s="7"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7"/>
+      <c r="E98" s="7"/>
     </row>
     <row r="99">
-      <c r="A99" s="6"/>
-      <c r="B99" s="6"/>
-      <c r="C99" s="6"/>
-      <c r="D99" s="6"/>
-      <c r="E99" s="6"/>
+      <c r="A99" s="7"/>
+      <c r="B99" s="7"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
     </row>
     <row r="100">
-      <c r="A100" s="6"/>
-      <c r="B100" s="6"/>
-      <c r="C100" s="6"/>
-      <c r="D100" s="6"/>
-      <c r="E100" s="6"/>
+      <c r="A100" s="7"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
+      <c r="E100" s="7"/>
     </row>
     <row r="101">
-      <c r="A101" s="6"/>
-      <c r="B101" s="6"/>
-      <c r="C101" s="6"/>
-      <c r="D101" s="6"/>
-      <c r="E101" s="6"/>
+      <c r="A101" s="7"/>
+      <c r="B101" s="7"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
     </row>
     <row r="102">
-      <c r="A102" s="6"/>
-      <c r="B102" s="6"/>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="6"/>
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7"/>
+      <c r="E102" s="7"/>
     </row>
     <row r="103">
       <c r="A103" s="11"/>

</xml_diff>